<commit_message>
TTH - đi dìa
</commit_message>
<xml_diff>
--- a/HD.xlsx
+++ b/HD.xlsx
@@ -5,34 +5,21 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\Zalo Received Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOWNLOAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" forceFullCalc="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="60">
   <si>
     <t>Mã Hợp Đồng</t>
   </si>
@@ -61,10 +48,13 @@
     <t>Ngày Phụ Lục</t>
   </si>
   <si>
-    <t>Giá Gốc</t>
-  </si>
-  <si>
-    <t>Giá Hiện Tại</t>
+    <t>Gía Gốc</t>
+  </si>
+  <si>
+    <t>Gía Hiện Tại</t>
+  </si>
+  <si>
+    <t>Số tài khoản</t>
   </si>
   <si>
     <t>Tên Chủ Tài Khoản</t>
@@ -79,6 +69,9 @@
     <t>Hợp Đồng</t>
   </si>
   <si>
+    <t>HD1</t>
+  </si>
+  <si>
     <t>TLM001</t>
   </si>
   <si>
@@ -97,7 +90,7 @@
     <t>2026-06-30</t>
   </si>
   <si>
-    <t>2023-05-30</t>
+    <t>2023-06-01</t>
   </si>
   <si>
     <t>Nguyễn Thị Huỳnh Cầm</t>
@@ -109,126 +102,113 @@
     <t>HD_Scan 1</t>
   </si>
   <si>
+    <t>HD10</t>
+  </si>
+  <si>
     <t>TLM002</t>
   </si>
   <si>
+    <t>CSHT_HUG_00119</t>
+  </si>
+  <si>
+    <t>Vi_Thuy_HUG</t>
+  </si>
+  <si>
+    <t>2023-05-01</t>
+  </si>
+  <si>
+    <t>2023-05-27</t>
+  </si>
+  <si>
+    <t>2023-06-06</t>
+  </si>
+  <si>
+    <t>Châu Thanh Nhã</t>
+  </si>
+  <si>
+    <t>BIDV CN Hậu Giang</t>
+  </si>
+  <si>
+    <t>HD_Scan 10</t>
+  </si>
+  <si>
+    <t>HD11</t>
+  </si>
+  <si>
+    <t>HD12</t>
+  </si>
+  <si>
     <t>DV2</t>
   </si>
   <si>
-    <t>CSHT_HUG_00119</t>
-  </si>
-  <si>
-    <t>Vi_Thuy_HUG</t>
-  </si>
-  <si>
-    <t>2023-05-01</t>
-  </si>
-  <si>
-    <t>2023-05-27</t>
-  </si>
-  <si>
-    <t>2023-05-23</t>
-  </si>
-  <si>
-    <t>Châu Thanh Nhã</t>
-  </si>
-  <si>
-    <t>BIDV CN Hậu Giang</t>
-  </si>
-  <si>
     <t>HD_Scan 2</t>
   </si>
   <si>
+    <t>HD17</t>
+  </si>
+  <si>
+    <t>NCT</t>
+  </si>
+  <si>
+    <t>HD18</t>
+  </si>
+  <si>
+    <t>HD2</t>
+  </si>
+  <si>
     <t>HD3</t>
   </si>
   <si>
-    <t>DV3</t>
-  </si>
-  <si>
     <t>HD_Scan 3</t>
   </si>
   <si>
     <t>HD4</t>
   </si>
   <si>
+    <t>HD_Scan 4</t>
+  </si>
+  <si>
     <t>HD5</t>
   </si>
   <si>
-    <t>DV4</t>
-  </si>
-  <si>
-    <t>DV5</t>
-  </si>
-  <si>
-    <t>HD_Scan 4</t>
-  </si>
-  <si>
     <t>HD_Scan 5</t>
   </si>
   <si>
     <t>HD6</t>
   </si>
   <si>
+    <t>HD_Scan 6</t>
+  </si>
+  <si>
     <t>HD7</t>
   </si>
   <si>
+    <t>HD_Scan 7</t>
+  </si>
+  <si>
     <t>HD8</t>
   </si>
   <si>
+    <t>HD_Scan 8</t>
+  </si>
+  <si>
     <t>HD9</t>
   </si>
   <si>
-    <t>HD10</t>
-  </si>
-  <si>
-    <t>DV6</t>
-  </si>
-  <si>
-    <t>DV7</t>
-  </si>
-  <si>
-    <t>DV8</t>
-  </si>
-  <si>
-    <t>DV9</t>
-  </si>
-  <si>
-    <t>DV10</t>
-  </si>
-  <si>
-    <t>HD_Scan 6</t>
-  </si>
-  <si>
-    <t>HD_Scan 7</t>
-  </si>
-  <si>
-    <t>HD_Scan 8</t>
-  </si>
-  <si>
-    <t>HD_Scan 10</t>
-  </si>
-  <si>
     <t>HD_Scan 9</t>
   </si>
   <si>
-    <t>HD11</t>
-  </si>
-  <si>
-    <t>HD12</t>
+    <t>https://drive.google.com/file/d/1tcuekDYEf7Wh6rdFZZzoEcWoMZIXK95z/view?usp=drive_link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -558,15 +538,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -612,34 +596,37 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J2">
         <v>1000000</v>
@@ -647,46 +634,49 @@
       <c r="K2">
         <v>1200000</v>
       </c>
-      <c r="L2" t="s">
-        <v>22</v>
+      <c r="L2">
+        <v>564654546</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="O2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J3">
         <v>20000000</v>
@@ -694,93 +684,99 @@
       <c r="K3">
         <v>22000000</v>
       </c>
-      <c r="L3" t="s">
-        <v>32</v>
+      <c r="L3">
+        <v>321321321</v>
       </c>
       <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
         <v>33</v>
       </c>
-      <c r="N3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="J4">
+        <v>1000000</v>
+      </c>
+      <c r="K4">
+        <v>1200000</v>
+      </c>
+      <c r="L4">
+        <v>2313211</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4">
-        <v>20000000</v>
-      </c>
-      <c r="K4">
-        <v>22000000</v>
-      </c>
-      <c r="L4" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" t="s">
-        <v>32</v>
-      </c>
       <c r="O4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J5">
         <v>20000000</v>
@@ -788,46 +784,49 @@
       <c r="K5">
         <v>22000000</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5">
+        <v>321231</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
         <v>32</v>
       </c>
-      <c r="M5" t="s">
+      <c r="I6" t="s">
         <v>33</v>
-      </c>
-      <c r="N5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" t="s">
-        <v>31</v>
       </c>
       <c r="J6">
         <v>20000000</v>
@@ -835,46 +834,49 @@
       <c r="K6">
         <v>22000000</v>
       </c>
-      <c r="L6" t="s">
-        <v>32</v>
+      <c r="L6">
+        <v>5313515315</v>
       </c>
       <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
         <v>33</v>
-      </c>
-      <c r="N6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" t="s">
-        <v>21</v>
       </c>
       <c r="J7">
         <v>1000000</v>
@@ -882,93 +884,99 @@
       <c r="K7">
         <v>1200000</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7">
+        <v>564654546</v>
+      </c>
+      <c r="M7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
         <v>22</v>
       </c>
-      <c r="M7" t="s">
+      <c r="I8" t="s">
         <v>23</v>
       </c>
-      <c r="N7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="J8">
+        <v>1000000</v>
+      </c>
+      <c r="K8">
+        <v>1200000</v>
+      </c>
+      <c r="L8">
+        <v>564654546</v>
+      </c>
+      <c r="M8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>45</v>
       </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="G8" t="s">
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="H8" t="s">
+      <c r="F9" t="s">
         <v>30</v>
       </c>
-      <c r="I8" t="s">
+      <c r="G9" t="s">
         <v>31</v>
       </c>
-      <c r="J8">
-        <v>20000000</v>
-      </c>
-      <c r="K8">
-        <v>22000000</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="H9" t="s">
         <v>32</v>
       </c>
-      <c r="M8" t="s">
+      <c r="I9" t="s">
         <v>33</v>
-      </c>
-      <c r="N8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" t="s">
-        <v>31</v>
       </c>
       <c r="J9">
         <v>20000000</v>
@@ -976,46 +984,49 @@
       <c r="K9">
         <v>22000000</v>
       </c>
-      <c r="L9" t="s">
-        <v>32</v>
+      <c r="L9">
+        <v>23152123</v>
       </c>
       <c r="M9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="O9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="P9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J10">
         <v>20000000</v>
@@ -1023,46 +1034,49 @@
       <c r="K10">
         <v>22000000</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10">
+        <v>66323131</v>
+      </c>
+      <c r="M10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" t="s">
         <v>32</v>
       </c>
-      <c r="M10" t="s">
+      <c r="I11" t="s">
         <v>33</v>
-      </c>
-      <c r="N10" t="s">
-        <v>32</v>
-      </c>
-      <c r="O10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" t="s">
-        <v>31</v>
       </c>
       <c r="J11">
         <v>20000000</v>
@@ -1070,21 +1084,224 @@
       <c r="K11">
         <v>22000000</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11">
+        <v>65343521</v>
+      </c>
+      <c r="M11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12">
+        <v>1000000</v>
+      </c>
+      <c r="K12">
+        <v>1200000</v>
+      </c>
+      <c r="L12">
+        <v>5312322</v>
+      </c>
+      <c r="M12" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" t="s">
         <v>32</v>
       </c>
-      <c r="M11" t="s">
+      <c r="I13" t="s">
         <v>33</v>
       </c>
-      <c r="N11" t="s">
+      <c r="J13">
+        <v>20000000</v>
+      </c>
+      <c r="K13">
+        <v>22000000</v>
+      </c>
+      <c r="L13">
+        <v>32121312</v>
+      </c>
+      <c r="M13" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" t="s">
         <v>32</v>
       </c>
-      <c r="O11" t="s">
+      <c r="I14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14">
+        <v>20000000</v>
+      </c>
+      <c r="K14">
+        <v>22000000</v>
+      </c>
+      <c r="L14">
+        <v>32513221</v>
+      </c>
+      <c r="M14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" t="s">
+        <v>34</v>
+      </c>
+      <c r="P14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>57</v>
       </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15">
+        <v>20000000</v>
+      </c>
+      <c r="K15">
+        <v>22000000</v>
+      </c>
+      <c r="L15">
+        <v>32132123</v>
+      </c>
+      <c r="M15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" t="s">
+        <v>34</v>
+      </c>
+      <c r="P15" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TTH - file HD
</commit_message>
<xml_diff>
--- a/HD.xlsx
+++ b/HD.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOWNLOAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huynp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13530" windowHeight="6315"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="63">
   <si>
     <t>Mã Hợp Đồng</t>
   </si>
@@ -199,6 +199,15 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1tcuekDYEf7Wh6rdFZZzoEcWoMZIXK95z/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Người Ký</t>
+  </si>
+  <si>
+    <t>Khách hàng</t>
+  </si>
+  <si>
+    <t>Trần Thị Hòa</t>
   </si>
 </sst>
 </file>
@@ -294,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -329,7 +338,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -538,19 +547,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="86.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -599,8 +615,14 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -649,8 +671,14 @@
       <c r="P2" t="s">
         <v>59</v>
       </c>
+      <c r="Q2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -699,8 +727,14 @@
       <c r="P3" t="s">
         <v>36</v>
       </c>
+      <c r="Q3" t="s">
+        <v>62</v>
+      </c>
+      <c r="R3" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -749,8 +783,14 @@
       <c r="P4" t="s">
         <v>26</v>
       </c>
+      <c r="Q4" t="s">
+        <v>62</v>
+      </c>
+      <c r="R4" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -799,8 +839,14 @@
       <c r="P5" t="s">
         <v>40</v>
       </c>
+      <c r="Q5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -849,8 +895,14 @@
       <c r="P6" t="s">
         <v>40</v>
       </c>
+      <c r="Q6" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -899,8 +951,14 @@
       <c r="P7" t="s">
         <v>26</v>
       </c>
+      <c r="Q7" t="s">
+        <v>62</v>
+      </c>
+      <c r="R7" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -949,8 +1007,14 @@
       <c r="P8" t="s">
         <v>26</v>
       </c>
+      <c r="Q8" t="s">
+        <v>62</v>
+      </c>
+      <c r="R8" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -999,8 +1063,14 @@
       <c r="P9" t="s">
         <v>46</v>
       </c>
+      <c r="Q9" t="s">
+        <v>62</v>
+      </c>
+      <c r="R9" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1049,8 +1119,14 @@
       <c r="P10" t="s">
         <v>48</v>
       </c>
+      <c r="Q10" t="s">
+        <v>62</v>
+      </c>
+      <c r="R10" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1099,8 +1175,14 @@
       <c r="P11" t="s">
         <v>50</v>
       </c>
+      <c r="Q11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R11" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1149,8 +1231,14 @@
       <c r="P12" t="s">
         <v>52</v>
       </c>
+      <c r="Q12" t="s">
+        <v>62</v>
+      </c>
+      <c r="R12" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1199,8 +1287,14 @@
       <c r="P13" t="s">
         <v>54</v>
       </c>
+      <c r="Q13" t="s">
+        <v>62</v>
+      </c>
+      <c r="R13" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1249,8 +1343,14 @@
       <c r="P14" t="s">
         <v>56</v>
       </c>
+      <c r="Q14" t="s">
+        <v>62</v>
+      </c>
+      <c r="R14" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -1298,6 +1398,12 @@
       </c>
       <c r="P15" t="s">
         <v>58</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>62</v>
+      </c>
+      <c r="R15" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>